<commit_message>
- fix: forgot to adjust the amount for two resistors
</commit_message>
<xml_diff>
--- a/D5035-01-20_ATSAME51/Project Outputs/D5035-01-20_BOM_Release.xlsx
+++ b/D5035-01-20_ATSAME51/Project Outputs/D5035-01-20_BOM_Release.xlsx
@@ -876,8 +876,8 @@
   </sheetPr>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.74609375" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1315,7 +1315,7 @@
         <v>12</v>
       </c>
       <c r="E15" s="7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>76</v>
@@ -1325,7 +1325,7 @@
       </c>
       <c r="H15" s="8" t="n">
         <f aca="false">E15*G15</f>
-        <v>0.475</v>
+        <v>0.38</v>
       </c>
       <c r="I15" s="8"/>
     </row>
@@ -1399,7 +1399,7 @@
         <v>21</v>
       </c>
       <c r="E18" s="7" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>85</v>
@@ -1409,7 +1409,7 @@
       </c>
       <c r="H18" s="8" t="n">
         <f aca="false">E18*G18</f>
-        <v>0.38</v>
+        <v>0.57</v>
       </c>
       <c r="I18" s="8"/>
     </row>
@@ -1750,7 +1750,7 @@
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H32" s="8" t="n">
         <f aca="false">SUM(H2:H31)</f>
-        <v>22.98</v>
+        <v>23.075</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>